<commit_message>
2. sprintin backlog päivitetty
</commit_message>
<xml_diff>
--- a/documents/Suunta_Sprint1_Backlog.xlsx
+++ b/documents/Suunta_Sprint1_Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>WHO</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -589,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,9 +667,6 @@
       <c r="E4" s="8">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -675,6 +675,12 @@
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -682,6 +688,12 @@
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Luokkakaavio ja backlog päivitetty
</commit_message>
<xml_diff>
--- a/documents/Suunta_Sprint1_Backlog.xlsx
+++ b/documents/Suunta_Sprint1_Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>WHO</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>Päivitetty:</t>
+  </si>
+  <si>
+    <t>(Mikko)</t>
   </si>
 </sst>
 </file>
@@ -206,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -251,6 +257,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +616,7 @@
     <col min="7" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
@@ -614,8 +624,17 @@
       <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="19">
+        <v>43066</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -628,7 +647,7 @@
       <c r="E2" s="9"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>20</v>
       </c>
@@ -651,7 +670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -668,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
@@ -679,10 +698,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
@@ -696,7 +715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
@@ -710,7 +729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -724,7 +743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
@@ -732,7 +751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>27</v>
       </c>
@@ -740,7 +759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Rest Api päivitetty, backlog päivitety, db-yhteys Mikon kantaan, andromedan insert-lauseet korjattu
</commit_message>
<xml_diff>
--- a/documents/Suunta_Sprint1_Backlog.xlsx
+++ b/documents/Suunta_Sprint1_Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>WHO</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>DONE</t>
-  </si>
-  <si>
-    <t>IN PROGRESS</t>
   </si>
   <si>
     <t>Päivitetty:</t>
@@ -603,7 +600,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,13 +622,13 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="19">
         <v>43066</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -712,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>